<commit_message>
📈 Intraday standard output (Mar–Sab)
</commit_message>
<xml_diff>
--- a/output/intraday/riepilogo_intraday_2026-01-14.xlsx
+++ b/output/intraday/riepilogo_intraday_2026-01-14.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW5"/>
+  <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -687,636 +687,952 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ATON</t>
+          <t>AHMA</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>46035</v>
       </c>
       <c r="C2" t="n">
-        <v>102.2</v>
+        <v>113.83</v>
       </c>
       <c r="D2" t="n">
-        <v>9910000</v>
+        <v>364030000</v>
       </c>
       <c r="E2" t="n">
-        <v>2820000</v>
+        <v>1920000</v>
       </c>
       <c r="F2" t="n">
-        <v>5740000</v>
+        <v>10740000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-29.35%</t>
+          <t>9.30%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>62.99</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.52</v>
-      </c>
+        <v>93.48999999999999</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
-        <v>8.779999999999999</v>
+        <v>0.41</v>
       </c>
       <c r="K2" t="n">
-        <v>1.84</v>
+        <v>10.96</v>
       </c>
       <c r="L2" t="n">
-        <v>1.93</v>
+        <v>11.22</v>
       </c>
       <c r="M2" t="n">
-        <v>3.3</v>
+        <v>13.83</v>
       </c>
       <c r="N2" t="n">
-        <v>1.53</v>
+        <v>8.82</v>
       </c>
       <c r="O2" t="n">
-        <v>1.99</v>
+        <v>12.31</v>
       </c>
       <c r="P2" t="n">
-        <v>369928550</v>
+        <v>83662202</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>2026-01-13 15:18:00</t>
+          <t>2026-01-13 14:59:00</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>2026-01-13 10:06:00</t>
+          <t>2026-01-13 09:58:00</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>2.34</v>
+        <v>5.15</v>
       </c>
       <c r="T2" t="n">
-        <v>2.43</v>
+        <v>15.21</v>
       </c>
       <c r="U2" t="n">
-        <v>1.97</v>
+        <v>5.07</v>
       </c>
       <c r="V2" t="n">
-        <v>2.16</v>
+        <v>11.3</v>
       </c>
       <c r="W2" t="n">
         <v>0</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>2026-01-13 05:01:00</t>
+          <t>2026-01-13 08:22:00</t>
         </is>
       </c>
       <c r="Y2" t="n">
-        <v>1.93</v>
+        <v>11.29</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.8</v>
+        <v>10.68</v>
       </c>
       <c r="AA2" t="n">
-        <v>15997031</v>
+        <v>22797890</v>
       </c>
       <c r="AB2" t="n">
-        <v>2.01</v>
+        <v>12.12</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.79</v>
+        <v>10.25</v>
       </c>
       <c r="AD2" t="n">
-        <v>16995816</v>
+        <v>23309466</v>
       </c>
       <c r="AE2" t="n">
-        <v>2.19</v>
+        <v>12.5</v>
       </c>
       <c r="AF2" t="n">
-        <v>1.72</v>
+        <v>8.82</v>
       </c>
       <c r="AG2" t="n">
-        <v>26661348</v>
+        <v>38114703</v>
       </c>
       <c r="AH2" t="n">
-        <v>2.19</v>
+        <v>12.5</v>
       </c>
       <c r="AI2" t="n">
-        <v>1.53</v>
+        <v>8.82</v>
       </c>
       <c r="AJ2" t="n">
-        <v>34033368</v>
+        <v>40297229</v>
       </c>
       <c r="AK2" t="n">
-        <v>1.81</v>
+        <v>10.38</v>
       </c>
       <c r="AL2" t="n">
-        <v>2.19</v>
+        <v>12.5</v>
       </c>
       <c r="AM2" t="n">
-        <v>1.53</v>
+        <v>8.82</v>
       </c>
       <c r="AN2" t="n">
-        <v>114822678</v>
+        <v>41373362</v>
       </c>
       <c r="AO2" t="n">
-        <v>1.73</v>
+        <v>10.21</v>
       </c>
       <c r="AP2" t="n">
-        <v>2.19</v>
+        <v>12.5</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1.53</v>
+        <v>8.82</v>
       </c>
       <c r="AR2" t="n">
-        <v>159586135</v>
+        <v>42011162</v>
       </c>
       <c r="AS2" t="n">
-        <v>1.91</v>
+        <v>11.23</v>
       </c>
       <c r="AT2" t="n">
-        <v>2.19</v>
+        <v>12.5</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.53</v>
+        <v>8.82</v>
       </c>
       <c r="AV2" t="n">
-        <v>215622491</v>
+        <v>61492984</v>
       </c>
       <c r="AW2" t="n">
-        <v>2.01</v>
+        <v>12.33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DCOY</t>
+          <t>ATON</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
         <v>46035</v>
       </c>
       <c r="C3" t="n">
-        <v>65.64</v>
+        <v>102.2</v>
       </c>
       <c r="D3" t="n">
-        <v>7980000</v>
+        <v>9910000</v>
       </c>
       <c r="E3" t="n">
-        <v>6000000</v>
+        <v>2820000</v>
       </c>
       <c r="F3" t="n">
-        <v>6380000</v>
+        <v>5740000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-7.41%</t>
+          <t>-29.35%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>6.05</v>
+        <v>62.99</v>
       </c>
       <c r="I3" t="n">
-        <v>4.71</v>
+        <v>0.52</v>
       </c>
       <c r="J3" t="n">
-        <v>3.08</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>1.24</v>
+        <v>1.88</v>
       </c>
       <c r="L3" t="n">
-        <v>1.28</v>
+        <v>1.82</v>
       </c>
       <c r="M3" t="n">
-        <v>1.36</v>
+        <v>3.3</v>
       </c>
       <c r="N3" t="n">
-        <v>1.07</v>
+        <v>1.53</v>
       </c>
       <c r="O3" t="n">
-        <v>1.23</v>
+        <v>1.99</v>
       </c>
       <c r="P3" t="n">
-        <v>799318234</v>
+        <v>385413301</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2026-01-13 14:23:00</t>
+          <t>2026-01-13 15:18:00</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>2026-01-13 09:53:00</t>
+          <t>2026-01-13 10:06:00</t>
         </is>
       </c>
       <c r="S3" t="n">
-        <v>0.8</v>
+        <v>2.59</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8</v>
+        <v>2.96</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8</v>
+        <v>1.81</v>
       </c>
       <c r="V3" t="n">
-        <v>0.8</v>
+        <v>1.81</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>2026-01-13 06:10:00</t>
+          <t>2026-01-13 08:04:00</t>
         </is>
       </c>
       <c r="Y3" t="n">
-        <v>1.31</v>
+        <v>1.93</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.21</v>
+        <v>1.77</v>
       </c>
       <c r="AA3" t="n">
-        <v>26848828</v>
+        <v>30969502</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.31</v>
+        <v>2.01</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.17</v>
+        <v>1.77</v>
       </c>
       <c r="AD3" t="n">
-        <v>28532761</v>
+        <v>32480567</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.31</v>
+        <v>2.19</v>
       </c>
       <c r="AF3" t="n">
-        <v>1.07</v>
+        <v>1.72</v>
       </c>
       <c r="AG3" t="n">
-        <v>36166989</v>
+        <v>42146099</v>
       </c>
       <c r="AH3" t="n">
-        <v>1.31</v>
+        <v>2.19</v>
       </c>
       <c r="AI3" t="n">
-        <v>1.07</v>
+        <v>1.53</v>
       </c>
       <c r="AJ3" t="n">
-        <v>158370115</v>
+        <v>49518119</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.23</v>
+        <v>1.81</v>
       </c>
       <c r="AL3" t="n">
-        <v>1.31</v>
+        <v>2.19</v>
       </c>
       <c r="AM3" t="n">
-        <v>1.07</v>
+        <v>1.53</v>
       </c>
       <c r="AN3" t="n">
-        <v>201871586</v>
+        <v>130307429</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.14</v>
+        <v>1.73</v>
       </c>
       <c r="AP3" t="n">
-        <v>1.31</v>
+        <v>2.19</v>
       </c>
       <c r="AQ3" t="n">
-        <v>1.07</v>
+        <v>1.53</v>
       </c>
       <c r="AR3" t="n">
-        <v>203979763</v>
+        <v>175070886</v>
       </c>
       <c r="AS3" t="n">
-        <v>1.17</v>
+        <v>1.91</v>
       </c>
       <c r="AT3" t="n">
-        <v>1.31</v>
+        <v>2.19</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.07</v>
+        <v>1.53</v>
       </c>
       <c r="AV3" t="n">
-        <v>335721281</v>
+        <v>231107242</v>
       </c>
       <c r="AW3" t="n">
-        <v>1.22</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EVTV</t>
+          <t>BCTX</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
         <v>46035</v>
       </c>
       <c r="C4" t="n">
-        <v>33.07</v>
+        <v>57.07</v>
       </c>
       <c r="D4" t="n">
-        <v>17000000</v>
+        <v>20530000</v>
       </c>
       <c r="E4" t="n">
-        <v>4450000</v>
+        <v>1860000</v>
       </c>
       <c r="F4" t="n">
-        <v>4830000</v>
+        <v>1880000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>5.39%</t>
+          <t>-9.00%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>7.9</v>
+        <v>1.27</v>
       </c>
       <c r="I4" t="n">
-        <v>1.91</v>
+        <v>1.67</v>
       </c>
       <c r="J4" t="n">
-        <v>0.97</v>
+        <v>15.13</v>
       </c>
       <c r="K4" t="n">
-        <v>3.15</v>
+        <v>11.65</v>
       </c>
       <c r="L4" t="n">
-        <v>3.15</v>
+        <v>11.96</v>
       </c>
       <c r="M4" t="n">
-        <v>4.91</v>
+        <v>12.1</v>
       </c>
       <c r="N4" t="n">
-        <v>2.62</v>
+        <v>9.06</v>
       </c>
       <c r="O4" t="n">
-        <v>3.52</v>
+        <v>11.15</v>
       </c>
       <c r="P4" t="n">
-        <v>407346086</v>
+        <v>12582674</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2026-01-13 13:34:00</t>
+          <t>2026-01-13 09:30:00</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>2026-01-13 09:54:00</t>
+          <t>2026-01-13 09:56:00</t>
         </is>
       </c>
       <c r="S4" t="n">
-        <v>3.2</v>
+        <v>8</v>
       </c>
       <c r="T4" t="n">
-        <v>3.5</v>
+        <v>19.68</v>
       </c>
       <c r="U4" t="n">
-        <v>2.88</v>
+        <v>7.82</v>
       </c>
       <c r="V4" t="n">
-        <v>3.4</v>
+        <v>12.27</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>2026-01-13 06:36:00</t>
+          <t>2026-01-13 08:12:00</t>
         </is>
       </c>
       <c r="Y4" t="n">
-        <v>3.25</v>
+        <v>12.1</v>
       </c>
       <c r="Z4" t="n">
-        <v>3.05</v>
+        <v>11.3</v>
       </c>
       <c r="AA4" t="n">
-        <v>16228048</v>
+        <v>3972208</v>
       </c>
       <c r="AB4" t="n">
-        <v>3.57</v>
+        <v>12.1</v>
       </c>
       <c r="AC4" t="n">
-        <v>2.95</v>
+        <v>10.41</v>
       </c>
       <c r="AD4" t="n">
-        <v>22346360</v>
+        <v>4027085</v>
       </c>
       <c r="AE4" t="n">
-        <v>3.57</v>
+        <v>12.1</v>
       </c>
       <c r="AF4" t="n">
-        <v>2.62</v>
+        <v>9.06</v>
       </c>
       <c r="AG4" t="n">
-        <v>35744132</v>
+        <v>4523387</v>
       </c>
       <c r="AH4" t="n">
-        <v>4.02</v>
+        <v>12.1</v>
       </c>
       <c r="AI4" t="n">
-        <v>2.62</v>
+        <v>9.06</v>
       </c>
       <c r="AJ4" t="n">
-        <v>61753960</v>
+        <v>4747625</v>
       </c>
       <c r="AK4" t="n">
-        <v>3.57</v>
+        <v>10.2</v>
       </c>
       <c r="AL4" t="n">
-        <v>4.02</v>
+        <v>12.1</v>
       </c>
       <c r="AM4" t="n">
-        <v>2.62</v>
+        <v>9.06</v>
       </c>
       <c r="AN4" t="n">
-        <v>76023072</v>
+        <v>4948881</v>
       </c>
       <c r="AO4" t="n">
-        <v>3.67</v>
+        <v>10.52</v>
       </c>
       <c r="AP4" t="n">
-        <v>4.02</v>
+        <v>12.1</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2.62</v>
+        <v>9.06</v>
       </c>
       <c r="AR4" t="n">
-        <v>147281895</v>
+        <v>5081171</v>
       </c>
       <c r="AS4" t="n">
-        <v>3.45</v>
+        <v>10.12</v>
       </c>
       <c r="AT4" t="n">
-        <v>4.87</v>
+        <v>12.1</v>
       </c>
       <c r="AU4" t="n">
-        <v>2.62</v>
+        <v>9.06</v>
       </c>
       <c r="AV4" t="n">
-        <v>269443112</v>
+        <v>5271397</v>
       </c>
       <c r="AW4" t="n">
-        <v>4.51</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>XAIR</t>
+          <t>DCOY</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
         <v>46035</v>
       </c>
       <c r="C5" t="n">
-        <v>79.22</v>
+        <v>65.64</v>
       </c>
       <c r="D5" t="n">
-        <v>17550000</v>
+        <v>7980000</v>
       </c>
       <c r="E5" t="n">
-        <v>7540000</v>
+        <v>6000000</v>
       </c>
       <c r="F5" t="n">
-        <v>8010000</v>
+        <v>6380000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>39.49%</t>
+          <t>-7.41%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>5.87</v>
+        <v>6.05</v>
       </c>
       <c r="I5" t="n">
-        <v>18.88</v>
+        <v>4.71</v>
       </c>
       <c r="J5" t="n">
-        <v>3.14</v>
+        <v>3.08</v>
       </c>
       <c r="K5" t="n">
-        <v>1.62</v>
+        <v>1.32</v>
       </c>
       <c r="L5" t="n">
-        <v>1.57</v>
+        <v>1.35</v>
       </c>
       <c r="M5" t="n">
-        <v>2.66</v>
+        <v>1.41</v>
       </c>
       <c r="N5" t="n">
-        <v>1.37</v>
+        <v>1.07</v>
       </c>
       <c r="O5" t="n">
-        <v>2.17</v>
+        <v>1.23</v>
       </c>
       <c r="P5" t="n">
-        <v>1366291685</v>
+        <v>825232430</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>2026-01-13 12:00:00</t>
+          <t>2026-01-13 09:30:00</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>2026-01-13 09:35:00</t>
+          <t>2026-01-13 09:53:00</t>
         </is>
       </c>
       <c r="S5" t="n">
-        <v>0.89</v>
+        <v>0.8</v>
       </c>
       <c r="T5" t="n">
-        <v>0.89</v>
+        <v>1.81</v>
       </c>
       <c r="U5" t="n">
-        <v>0.89</v>
+        <v>0.77</v>
       </c>
       <c r="V5" t="n">
-        <v>0.89</v>
+        <v>1.36</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>2026-01-13 05:41:00</t>
+          <t>2026-01-13 08:43:00</t>
         </is>
       </c>
       <c r="Y5" t="n">
-        <v>1.68</v>
+        <v>1.41</v>
       </c>
       <c r="Z5" t="n">
-        <v>1.56</v>
+        <v>1.26</v>
       </c>
       <c r="AA5" t="n">
-        <v>31709159</v>
+        <v>51828392</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.68</v>
+        <v>1.41</v>
       </c>
       <c r="AC5" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>54446957</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>62081185</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>184284311</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>227785782</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>229893959</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>361635477</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>EVTV</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>46035</v>
+      </c>
+      <c r="C6" t="n">
+        <v>33.07</v>
+      </c>
+      <c r="D6" t="n">
+        <v>17000000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4450000</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4830000</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>5.39%</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="L6" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="P6" t="n">
+        <v>422796722</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2026-01-13 13:34:00</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2026-01-13 09:54:00</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="T6" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="V6" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>2026-01-13 08:02:00</t>
+        </is>
+      </c>
+      <c r="Y6" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>30901272</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>37796996</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>51194768</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>77204596</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>91473708</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>162732531</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>284893748</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>XAIR</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>46035</v>
+      </c>
+      <c r="C7" t="n">
+        <v>79.22</v>
+      </c>
+      <c r="D7" t="n">
+        <v>17550000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7540000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8010000</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>39.49%</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="I7" t="n">
+        <v>18.88</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="O7" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1396493630</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>2026-01-13 12:00:00</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>2026-01-13 09:35:00</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="V7" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>2026-01-13 09:19:00</t>
+        </is>
+      </c>
+      <c r="Y7" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="Z7" t="n">
         <v>1.55</v>
       </c>
-      <c r="AD5" t="n">
-        <v>34613205</v>
-      </c>
-      <c r="AE5" t="n">
+      <c r="AA7" t="n">
+        <v>60403890</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>64815150</v>
+      </c>
+      <c r="AE7" t="n">
         <v>2.04</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AF7" t="n">
         <v>1.37</v>
       </c>
-      <c r="AG5" t="n">
-        <v>253653902</v>
-      </c>
-      <c r="AH5" t="n">
+      <c r="AG7" t="n">
+        <v>283855847</v>
+      </c>
+      <c r="AH7" t="n">
         <v>2.5</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AI7" t="n">
         <v>1.37</v>
       </c>
-      <c r="AJ5" t="n">
-        <v>369562619</v>
-      </c>
-      <c r="AK5" t="n">
+      <c r="AJ7" t="n">
+        <v>399764564</v>
+      </c>
+      <c r="AK7" t="n">
         <v>2.38</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="AL7" t="n">
         <v>2.5</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AM7" t="n">
         <v>1.37</v>
       </c>
-      <c r="AN5" t="n">
-        <v>498063712</v>
-      </c>
-      <c r="AO5" t="n">
+      <c r="AN7" t="n">
+        <v>528265657</v>
+      </c>
+      <c r="AO7" t="n">
         <v>2.2</v>
       </c>
-      <c r="AP5" t="n">
+      <c r="AP7" t="n">
         <v>2.5</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="AQ7" t="n">
         <v>1.37</v>
       </c>
-      <c r="AR5" t="n">
-        <v>509913327</v>
-      </c>
-      <c r="AS5" t="n">
+      <c r="AR7" t="n">
+        <v>540115272</v>
+      </c>
+      <c r="AS7" t="n">
         <v>2.51</v>
       </c>
-      <c r="AT5" t="n">
+      <c r="AT7" t="n">
         <v>2.66</v>
       </c>
-      <c r="AU5" t="n">
+      <c r="AU7" t="n">
         <v>1.37</v>
       </c>
-      <c r="AV5" t="n">
-        <v>848594462</v>
-      </c>
-      <c r="AW5" t="n">
+      <c r="AV7" t="n">
+        <v>878796407</v>
+      </c>
+      <c r="AW7" t="n">
         <v>2.34</v>
       </c>
     </row>

</xml_diff>